<commit_message>
Updated and added even more specific tests
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_junction_test.xlsx
+++ b/tests/frameworks/framework_junction_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855AAD82-BF2D-40C8-84FC-3345FD02E889}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8B7D82-33F0-4006-B845-2814037DD033}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Transitions" sheetId="3" r:id="rId3"/>
     <sheet name="Characteristics" sheetId="4" r:id="rId4"/>
     <sheet name="Parameters" sheetId="6" r:id="rId5"/>
-    <sheet name="Interactions" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
@@ -539,77 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{F7DF6DA5-307D-42BB-80B5-CEE9AB8ED752}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'min' attribute for a 'par' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{4C3AB2C0-9D0C-4C0E-9CF0-D571224FE5BD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'max' attribute for a 'par' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{98B9E77F-8634-4220-9AE2-2EB54A125949}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'func' attribute for a 'par' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{974FC231-C2BA-4000-88CD-AB6CE23C45D0}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for tagging a parameter as a potential program
-impact.
-Note: This tag is only enabled for a parameter by marking the
-corresponding cell 'y'.
-Anything else, including keeping the cell blank, disables the tag.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{56CE2189-0A42-47B2-BD42-8E8BFBCF4F01}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column marks whether parameter data can be rescaled
-during model calibration processes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{9AB3D83C-D0BC-4583-B5B1-006FE7C2562F}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9AB3D83C-D0BC-4583-B5B1-006FE7C2562F}">
       <text>
         <r>
           <rPr>
@@ -628,99 +557,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{F4694702-1A69-4233-A84B-A75E88284228}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column currently denotes whether a databook should request
-historical values from the user for this parameter.
-A value of '-1' suppresses it from appearing in the databook.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{162B0863-E71C-4603-A693-15E6A2B23038}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for the 'code name' of a population interaction.
-These are special parameters that do not store values per population
-but per pairs of populations, specifically relating to how a source
-population interacts with a target population.
-Examples may include 'w_ctc', 'sex_partners', etc.
-The values that users provide for these matrix parameters, possibly
-time-dependent, can be propagated into population parameters by
-special functions such as 'srcpopavg'.
-Refer to documentation for more details.
-Note: A display name is a representative label that users interface
-with (e.g. in databooks and plots).
-It should be in title or sentence case.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{FC00BD5D-BBD8-48DF-8AE7-162658709D7A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for the 'display name' of a population interaction.
-These are special parameters that do not store values per population
-but per pairs of populations, specifically relating to how a source
-population interacts with a target population.
-Examples may include 'Contact weighting', 'Number of sex partners',
-etc.
-The values that users provide for these matrix parameters, possibly
-time-dependent, can be propagated into population parameters by
-special functions such as 'srcpopavg'.
-Refer to documentation for more details.
-Note: A display name is a representative label that users interface
-with (e.g. in databooks and plots).
-It should be in title or sentence case.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{ED07D9E4-694E-4387-BFA2-CAB6F8A058EC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'default_value' attribute for a 'interpop' item.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="56">
   <si>
     <t>Datasheet Code Name</t>
   </si>
@@ -765,18 +607,6 @@
   </si>
   <si>
     <t>Format</t>
-  </si>
-  <si>
-    <t>Minimum Value</t>
-  </si>
-  <si>
-    <t>Maximum Value</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Is Impact</t>
   </si>
   <si>
     <t>parameters</t>
@@ -895,6 +725,12 @@
   <si>
     <t>proportion</t>
   </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>Flow src to C</t>
+  </si>
 </sst>
 </file>
 
@@ -981,7 +817,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1034,20 +877,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1062,7 +891,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1446,23 +1275,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1478,7 +1307,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,13 +1361,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1548,10 +1377,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
@@ -1559,80 +1388,80 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
@@ -1640,17 +1469,17 @@
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
@@ -1658,17 +1487,17 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
@@ -1676,46 +1505,46 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I1048576">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>AND(J4&lt;&gt;"",NOT(I4&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1725,7 +1554,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A10">
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>AND(#REF!&lt;&gt;"",NOT(A3&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1777,7 +1606,7 @@
   <dimension ref="A1:OH398"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,37 +1616,37 @@
   <sheetData>
     <row r="1" spans="1:398" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="K1" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L1" s="3" t="str">
         <f>IF(Compartments!$A19&lt;&gt;"",Compartments!$A19,"")</f>
@@ -3370,88 +3199,91 @@
     </row>
     <row r="2" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:398" x14ac:dyDescent="0.25">
@@ -5778,7 +5610,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:J1">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>AND(B1&lt;&gt;"",NOT(C1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5873,12 +5705,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(A2&lt;&gt;"",NOT(B2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND(I2&lt;&gt;"",NOT(H2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5927,10 +5759,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5939,15 +5771,10 @@
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="7" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5961,198 +5788,191 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D2" s="7">
         <v>100</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D4" s="7">
         <v>0.5</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D5" s="7">
         <v>0.5</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D6" s="7">
         <v>0.5</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D7" s="7">
         <v>0.5</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
         <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>57</v>
       </c>
       <c r="D8" s="7">
         <v>0.5</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D9" s="7">
         <v>0.5</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>19</v>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="7">
+        <v>100</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>AND(K2&lt;&gt;"",NOT(J2&lt;&gt;""))</formula>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>AND(#REF!&lt;&gt;"",NOT(E2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:I1048576" xr:uid="{7CB7BECB-8CCA-402C-8209-B57AEC65D6EC}">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Code names must be unique" error="Parameter code names must be unique" sqref="A1:A1048576" xr:uid="{E6E68E87-C2E4-4D80-BD6F-D69CE5F2A8E2}">
       <formula1>COUNTIF(A:A,A1)&lt;2</formula1>
     </dataValidation>
@@ -6164,7 +5984,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{BE3DBFB1-F6C9-4726-B787-A3DD602656FE}">
-            <xm:f>AND(J2&lt;&gt;"",ISERROR(MATCH(J2,'Databook Pages'!$A:$A,0)))</xm:f>
+            <xm:f>AND(E2&lt;&gt;"",ISERROR(MATCH(E2,'Databook Pages'!$A:$A,0)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -6173,7 +5993,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6183,51 +6003,10 @@
           <x14:formula1>
             <xm:f>'Databook Pages'!$A$2:$A$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Tidy up tests, they all run now
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_junction_test.xlsx
+++ b/tests/frameworks/framework_junction_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8B7D82-33F0-4006-B845-2814037DD033}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F075D6-4491-4473-8C4C-A46C8C0B9E4B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,13 @@
     <sheet name="Parameters" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -636,31 +643,7 @@
     <t>Sink</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
   </si>
   <si>
     <t>jb1</t>
@@ -730,6 +713,30 @@
   </si>
   <si>
     <t>Flow src to C</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>cb</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>ce</t>
+  </si>
+  <si>
+    <t>cf</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>ch</t>
   </si>
 </sst>
 </file>
@@ -817,7 +824,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1291,7 +1319,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1306,8 +1334,8 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,7 +1395,7 @@
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1377,10 +1405,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
@@ -1395,13 +1423,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
@@ -1416,13 +1444,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
@@ -1437,13 +1465,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
@@ -1458,10 +1486,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
@@ -1476,10 +1504,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
@@ -1494,10 +1522,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
@@ -1512,10 +1540,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
@@ -1533,29 +1561,34 @@
         <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="12" priority="5">
+  <conditionalFormatting sqref="B1:B2 B11:B1048576">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I1048576">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>AND(J4&lt;&gt;"",NOT(I4&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I10">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="13" priority="10">
       <formula>AND(J2&lt;&gt;"",NOT(I3&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A10">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>AND(#REF!&lt;&gt;"",NOT(A3&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B10">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>AND(#REF!&lt;&gt;"",NOT(B3&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1570,7 +1603,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{0238372B-F012-4B98-A58B-305EDC0BD903}">
+          <x14:cfRule type="expression" priority="3" id="{0238372B-F012-4B98-A58B-305EDC0BD903}">
             <xm:f>AND(I3&lt;&gt;"",ISERROR(MATCH(I3,'Databook Pages'!$A:$A,0)))</xm:f>
             <x14:dxf>
               <fill>
@@ -1605,8 +1638,8 @@
   </sheetPr>
   <dimension ref="A1:OH398"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,28 +1655,28 @@
         <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>21</v>
@@ -3202,83 +3235,83 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="K8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:398" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="K10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:398" x14ac:dyDescent="0.25">
@@ -5609,19 +5642,24 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A3:A10">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(#REF!&lt;&gt;"",NOT(A3&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C1:J1">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>AND(B1&lt;&gt;"",NOT(C1&lt;&gt;""))</formula>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(#REF!&lt;&gt;"",NOT(C1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{51D293C8-E19A-4195-82DA-432679B2823C}">
+          <x14:cfRule type="expression" priority="4" id="{51D293C8-E19A-4195-82DA-432679B2823C}">
             <xm:f>AND(B2&lt;&gt;"",ISERROR(MATCH(B2,Parameters!$A:$A,0)))</xm:f>
             <x14:dxf>
               <fill>
@@ -5705,12 +5743,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>AND(A2&lt;&gt;"",NOT(B2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>AND(I2&lt;&gt;"",NOT(H2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5793,13 +5831,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D2" s="7">
         <v>100</v>
@@ -5810,13 +5848,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
@@ -5827,13 +5865,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
       </c>
       <c r="D4" s="7">
         <v>0.5</v>
@@ -5844,13 +5882,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D5" s="7">
         <v>0.5</v>
@@ -5861,13 +5899,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D6" s="7">
         <v>0.5</v>
@@ -5878,13 +5916,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D7" s="7">
         <v>0.5</v>
@@ -5895,13 +5933,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D8" s="7">
         <v>0.5</v>
@@ -5912,13 +5950,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7">
         <v>0.5</v>
@@ -5929,13 +5967,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
@@ -5946,13 +5984,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7">
         <v>100</v>
@@ -5963,12 +6001,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(A1&lt;&gt;"",NOT(B1&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="expression" dxfId="1" priority="11">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>AND(#REF!&lt;&gt;"",NOT(E2&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>